<commit_message>
add scene.js and relationships.js
</commit_message>
<xml_diff>
--- a/doc/log/log_201608040102_weixinxin.xlsx
+++ b/doc/log/log_201608040102_weixinxin.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46">
   <si>
     <t>时间</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>编写MyObject视图</t>
+  </si>
+  <si>
+    <t>编写scene js</t>
   </si>
 </sst>
 </file>
@@ -157,10 +160,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -173,6 +176,29 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,29 +235,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -252,35 +255,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -309,7 +283,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,19 +327,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,60 +375,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -420,13 +441,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,72 +508,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,6 +575,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -595,26 +618,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -623,10 +626,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -635,133 +638,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1123,7 +1126,7 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+      <selection activeCell="E60" sqref="E60:F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1986,13 +1989,21 @@
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="C58" s="1">
+        <v>6.26</v>
+      </c>
       <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="G58" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>

</xml_diff>